<commit_message>
SK-3: manga artiklar + SK-4: langa kommentarer + SK-6: centrera antal + SK-16: ny produktlista
</commit_message>
<xml_diff>
--- a/templates/pack_list_template.xlsx
+++ b/templates/pack_list_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atw10wp4\Jupyter\Enterprise\SvenskaKyrkan\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEBF1C8-A302-45CE-9958-4D914C291714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E769A1-B429-4D83-AF6C-D4DBB2CCBD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -443,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1"/>
@@ -482,9 +482,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -517,6 +514,12 @@
     <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,18 +532,27 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,88 +864,88 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="41" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="41" customWidth="1"/>
-    <col min="3" max="3" width="6.109375" style="41" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" style="41" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" style="41" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" style="41" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="41" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" style="41" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" style="41" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="41" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" style="41" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="40" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="40" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" style="40" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="40" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="40" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="40" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="40" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="40" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="38"/>
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="37"/>
+      <c r="B1" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="47" t="s">
+      <c r="G1" s="42"/>
+      <c r="H1" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="44" t="s">
+      <c r="I1" s="49"/>
+      <c r="J1" s="43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+    <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="50" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
     </row>
-    <row r="3" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+    <row r="3" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
-    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="55"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="7"/>
       <c r="F4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="39" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="19" t="s">
@@ -942,7 +954,7 @@
       <c r="I4" s="10"/>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
@@ -969,37 +981,37 @@
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="59" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="53"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="52"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="56"/>
     </row>
-    <row r="7" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="37"/>
+    <row r="7" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="30"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="36"/>
     </row>
-    <row r="8" spans="1:11" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="20" t="s">
         <v>16</v>
@@ -1013,7 +1025,7 @@
       <c r="I9" s="21"/>
       <c r="J9" s="22"/>
     </row>
-    <row r="10" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="B10" s="23" t="s">
         <v>17</v>
@@ -1031,7 +1043,7 @@
       <c r="I10" s="27"/>
       <c r="J10" s="29"/>
     </row>
-    <row r="11" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="23" t="s">
         <v>20</v>
@@ -1051,7 +1063,7 @@
       </c>
       <c r="J11" s="28"/>
     </row>
-    <row r="12" spans="1:11" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>

</xml_diff>

<commit_message>
SK-19: utan produktlista + SK-12: ändrad titel + SK-7: slutruta
</commit_message>
<xml_diff>
--- a/templates/pack_list_template.xlsx
+++ b/templates/pack_list_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atw10wp4\Jupyter\Enterprise\SvenskaKyrkan\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E769A1-B429-4D83-AF6C-D4DBB2CCBD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8037A4F1-E5EE-45FC-9441-0E666A74CFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Total:</t>
   </si>
@@ -94,15 +94,9 @@
     <t>Kurzbeschreibung</t>
   </si>
   <si>
-    <t>Preis</t>
-  </si>
-  <si>
     <t>Antal Påsar:</t>
   </si>
   <si>
-    <t>Pynt</t>
-  </si>
-  <si>
     <t>Sverige</t>
   </si>
   <si>
@@ -118,9 +112,6 @@
     <t>Paulaner</t>
   </si>
   <si>
-    <t>Frys:</t>
-  </si>
-  <si>
     <t>Full Name</t>
   </si>
   <si>
@@ -134,15 +125,22 @@
   </si>
   <si>
     <t>Ant.Orderrader</t>
+  </si>
+  <si>
+    <t>Semlor</t>
+  </si>
+  <si>
+    <t>Frys</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-[$€-C07]\ * #,##0.00_-;\-[$€-C07]\ * #,##0.00_-;_-[$€-C07]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="hh:mm;@"/>
+    <numFmt numFmtId="168" formatCode="[$€-2]\ #,##0.00"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -460,9 +458,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyBorder="1"/>
@@ -520,6 +515,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,9 +549,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="168" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,44 +860,44 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="40" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="40" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="40" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="40" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" style="40" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="40" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" style="40" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="40" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" style="40" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="40" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="40" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="39" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="39" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" style="39" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="39" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="39" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" style="39" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="39" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="39" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="39" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="37"/>
+      <c r="A1" s="36"/>
       <c r="B1" s="46" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C1" s="47"/>
       <c r="D1" s="47"/>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="42"/>
+      <c r="F1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="41"/>
       <c r="H1" s="48" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I1" s="49"/>
-      <c r="J1" s="43" t="s">
-        <v>27</v>
+      <c r="J1" s="42" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -921,16 +917,16 @@
       <c r="J2" s="53"/>
     </row>
     <row r="3" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
@@ -943,12 +939,12 @@
       <c r="D4" s="58"/>
       <c r="E4" s="7"/>
       <c r="F4" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="18" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="10"/>
@@ -975,22 +971,22 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18">
+      <c r="A6" s="17">
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="44" t="s">
+      <c r="E6" s="59">
+        <v>11</v>
+      </c>
+      <c r="F6" s="43" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="54"/>
@@ -999,81 +995,81 @@
       <c r="J6" s="56"/>
     </row>
     <row r="7" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="36"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:11" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
-      <c r="B9" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="22"/>
+      <c r="B9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="29"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="28"/>
     </row>
     <row r="11" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="28"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="17"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1085,6 +1081,6 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.31496062992125978" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
-  <pageSetup paperSize="9" scale="76" fitToHeight="0" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="76" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SK-20: templates större typsnitt
</commit_message>
<xml_diff>
--- a/templates/pack_list_template.xlsx
+++ b/templates/pack_list_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atw10wp4\Jupyter\Enterprise\SvenskaKyrkan\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8037A4F1-E5EE-45FC-9441-0E666A74CFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10668574-3221-4EE8-ABEE-D4470C4A3F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -140,7 +140,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-[$€-C07]\ * #,##0.00_-;\-[$€-C07]\ * #,##0.00_-;_-[$€-C07]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="hh:mm;@"/>
-    <numFmt numFmtId="168" formatCode="[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="166" formatCode="[$€-2]\ #,##0.00"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -549,7 +549,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,25 +860,25 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="39" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="39" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="39" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="39" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="39" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" style="39" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="39" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="39" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="39" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="39" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" style="39" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="39" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" style="39" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" style="39" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="39" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" style="39" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="39" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="39" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" style="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="36"/>
       <c r="B1" s="46" t="s">
         <v>21</v>
@@ -900,7 +900,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
@@ -916,7 +916,7 @@
       <c r="I2" s="52"/>
       <c r="J2" s="53"/>
     </row>
-    <row r="3" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
@@ -928,7 +928,7 @@
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
     </row>
-    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
         <v>3</v>
@@ -950,7 +950,7 @@
       <c r="I4" s="10"/>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
@@ -970,7 +970,7 @@
       <c r="H5" s="1"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="17">
         <v>1</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="I6" s="55"/>
       <c r="J6" s="56"/>
     </row>
-    <row r="7" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29"/>
       <c r="B7" s="30"/>
       <c r="C7" s="31"/>
@@ -1006,8 +1006,8 @@
       <c r="I7" s="34"/>
       <c r="J7" s="35"/>
     </row>
-    <row r="8" spans="1:11" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
       <c r="B9" s="19" t="s">
         <v>15</v>
@@ -1021,7 +1021,7 @@
       <c r="I9" s="20"/>
       <c r="J9" s="21"/>
     </row>
-    <row r="10" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="22" t="s">
         <v>26</v>
@@ -1039,7 +1039,7 @@
       <c r="I10" s="26"/>
       <c r="J10" s="28"/>
     </row>
-    <row r="11" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="22" t="s">
         <v>18</v>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="J11" s="27"/>
     </row>
-    <row r="12" spans="1:11" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="9.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>

</xml_diff>